<commit_message>
modify ClimaWatch Defect Report, ClimaWatch Testing Documentation, and add ClimaWatch Test Report
</commit_message>
<xml_diff>
--- a/ClimaWatch Defect Report.xlsx
+++ b/ClimaWatch Defect Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Super\Revature\Project 2\BKDS\ClimaWatch Testing Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B6FBC6-E1B8-4F33-93B5-787AFB94543F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29A1F5-2D04-4FD1-832A-ED131ED3E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34DF1769-5401-4AFD-9EB8-EA18261C005A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>ClimaWatch Bug Tracking</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Steps to Reproduce if Requried</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
   </si>
   <si>
     <t>Severity</t>
-  </si>
-  <si>
-    <t>Testers comments</t>
-  </si>
-  <si>
-    <t>Developer comments</t>
   </si>
   <si>
     <t>M-1</t>
@@ -236,9 +227,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -247,6 +235,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7733CB4F-0AB2-4889-821E-4B479A2A39E1}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,35 +565,29 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="52.44140625" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="34" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="12" width="10.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,19 +619,10 @@
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -654,37 +630,34 @@
         <v>44775</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -692,37 +665,34 @@
         <v>44776</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -730,37 +700,34 @@
         <v>44777</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
+      <c r="F5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -768,37 +735,34 @@
         <v>44781</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -806,37 +770,34 @@
         <v>44781</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -844,37 +805,34 @@
         <v>44784</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -882,37 +840,34 @@
         <v>44785</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -924,13 +879,10 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
modify ClimaWatch Defect Report.xlsx
</commit_message>
<xml_diff>
--- a/ClimaWatch Defect Report.xlsx
+++ b/ClimaWatch Defect Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Super\Revature\Project 2\BKDS\ClimaWatch Testing Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F29A1F5-2D04-4FD1-832A-ED131ED3E7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D25E483-12C0-43BC-B1FD-8B52DE8DCE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34DF1769-5401-4AFD-9EB8-EA18261C005A}"/>
+    <workbookView xWindow="5760" yWindow="2328" windowWidth="17280" windowHeight="8964" xr2:uid="{34DF1769-5401-4AFD-9EB8-EA18261C005A}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Report" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="43">
   <si>
     <t>ClimaWatch Bug Tracking</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Clock display was showing AM when current time was PM</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Content</t>
@@ -177,17 +174,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,9 +222,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -573,19 +560,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -619,7 +606,7 @@
         <v>10</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -651,7 +638,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>21</v>
@@ -686,7 +673,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>26</v>
@@ -721,7 +708,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>21</v>
@@ -756,7 +743,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>26</v>
@@ -775,8 +762,8 @@
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>32</v>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
@@ -788,13 +775,13 @@
         <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -808,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>16</v>
@@ -820,13 +807,13 @@
         <v>18</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>21</v>
@@ -840,13 +827,13 @@
         <v>44785</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>23</v>
@@ -855,13 +842,13 @@
         <v>18</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>26</v>

</xml_diff>